<commit_message>
DOCS: Atualização da documentação do projeto
</commit_message>
<xml_diff>
--- a/notebook/resultados_algoritmos.xlsx
+++ b/notebook/resultados_algoritmos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>name</t>
   </si>
@@ -28,10 +28,22 @@
     <t>XGB - Extreme Boosting Classifier</t>
   </si>
   <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>SVM - Support Vector Machine</t>
+  </si>
+  <si>
     <t>StandardScaler</t>
   </si>
   <si>
     <t>RobustScaler</t>
+  </si>
+  <si>
+    <t>PowerTransformer</t>
+  </si>
+  <si>
+    <t>MinMaxScaler</t>
   </si>
   <si>
     <t>Normalizer</t>
@@ -392,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,10 +426,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>80.25</v>
+        <v>83.44</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -425,10 +437,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>80.25</v>
+        <v>83.44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -436,10 +448,142 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>83.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>83.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>72.51000000000001</v>
+      <c r="C6">
+        <v>82.72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>82.42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>81.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>80.77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>76.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>76.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>75.29000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>73.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>72.19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>71.01000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>70.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>